<commit_message>
add comment for codes
</commit_message>
<xml_diff>
--- a/src/test/java/seatech/uiTest/ibv/testcase/TC_Ck trong.xlsx
+++ b/src/test/java/seatech/uiTest/ibv/testcase/TC_Ck trong.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\automation-test-master\src\test\java\seatech\uiTest\ibv\testcase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49FAD80-6881-47C5-9676-6FC042667DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7EC1684-2980-4D23-8047-58ED265FD02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -531,7 +531,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -696,46 +696,9 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1024,7 +987,7 @@
   <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1445,7 +1408,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="40" t="s">
         <v>57</v>
       </c>
@@ -1486,7 +1449,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="70" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>7</v>
       </c>
@@ -1729,7 +1692,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" s="40" t="s">
         <v>57</v>
       </c>
@@ -2033,7 +1996,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="40" t="s">
         <v>57</v>
       </c>
@@ -3054,188 +3017,187 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.375" style="57" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.25" style="57" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.375" style="57" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.75" style="57" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="11" style="57"/>
+    <col min="1" max="1" width="4.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.75" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="56"/>
       <c r="B1" s="56"/>
       <c r="C1" s="56"/>
       <c r="D1" s="56"/>
       <c r="E1" s="56"/>
     </row>
-    <row r="2" spans="1:5" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="56"/>
       <c r="B2" s="56"/>
       <c r="C2" s="56"/>
       <c r="D2" s="56"/>
       <c r="E2" s="56"/>
     </row>
-    <row r="3" spans="1:5" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="56"/>
       <c r="B3" s="56"/>
       <c r="C3" s="56"/>
       <c r="D3" s="56"/>
       <c r="E3" s="56"/>
     </row>
-    <row r="4" spans="1:5" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="56"/>
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
       <c r="D4" s="56"/>
       <c r="E4" s="56"/>
     </row>
-    <row r="5" spans="1:5" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="56"/>
       <c r="B5" s="56"/>
       <c r="C5" s="56"/>
       <c r="D5" s="56"/>
       <c r="E5" s="56"/>
     </row>
-    <row r="6" spans="1:5" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="56"/>
       <c r="B6" s="56"/>
       <c r="C6" s="56"/>
       <c r="D6" s="56"/>
       <c r="E6" s="56"/>
     </row>
-    <row r="7" spans="1:5" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="56"/>
       <c r="B7" s="56"/>
       <c r="C7" s="56"/>
       <c r="D7" s="56"/>
       <c r="E7" s="56"/>
     </row>
-    <row r="8" spans="1:5" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="56"/>
       <c r="B8" s="56"/>
       <c r="C8" s="56"/>
       <c r="D8" s="56"/>
       <c r="E8" s="56"/>
     </row>
-    <row r="9" spans="1:5" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="56"/>
       <c r="B9" s="56"/>
       <c r="C9" s="56"/>
       <c r="D9" s="56"/>
       <c r="E9" s="56"/>
     </row>
-    <row r="10" spans="1:5" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="56"/>
       <c r="B10" s="56"/>
       <c r="C10" s="56"/>
       <c r="D10" s="56"/>
       <c r="E10" s="56"/>
     </row>
-    <row r="11" spans="1:5" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="56"/>
       <c r="B11" s="56"/>
       <c r="C11" s="56"/>
       <c r="D11" s="56"/>
       <c r="E11" s="56"/>
     </row>
-    <row r="51" spans="1:7" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="58"/>
-      <c r="B51" s="59"/>
-      <c r="C51" s="58"/>
-      <c r="D51" s="60"/>
-      <c r="E51" s="58"/>
-      <c r="F51" s="61"/>
-      <c r="G51" s="58"/>
-    </row>
-    <row r="52" spans="1:7" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="58"/>
-      <c r="B52" s="59"/>
-      <c r="C52" s="58"/>
-      <c r="D52" s="61"/>
-      <c r="E52" s="58"/>
-      <c r="F52" s="61"/>
-      <c r="G52" s="58"/>
-    </row>
-    <row r="53" spans="1:7" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="58"/>
-      <c r="B53" s="59"/>
-      <c r="C53" s="58"/>
-      <c r="D53" s="60"/>
-      <c r="E53" s="58"/>
-      <c r="F53" s="61"/>
-      <c r="G53" s="58"/>
-    </row>
-    <row r="54" spans="1:7" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="58"/>
-      <c r="B54" s="59"/>
-      <c r="C54" s="58"/>
-      <c r="D54" s="61"/>
-      <c r="E54" s="58"/>
-      <c r="F54" s="63"/>
-      <c r="G54" s="58"/>
-    </row>
-    <row r="55" spans="1:7" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="58"/>
-      <c r="B55" s="59"/>
-      <c r="C55" s="58"/>
-      <c r="D55" s="61"/>
-      <c r="E55" s="58"/>
-      <c r="F55" s="64"/>
-      <c r="G55" s="58"/>
-    </row>
-    <row r="56" spans="1:7" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="58"/>
-      <c r="B56" s="59"/>
-      <c r="C56" s="58"/>
-      <c r="D56" s="65"/>
-      <c r="E56" s="58"/>
-      <c r="F56" s="64"/>
-      <c r="G56" s="58"/>
-    </row>
-    <row r="57" spans="1:7" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="58"/>
-      <c r="B57" s="59"/>
-      <c r="C57" s="58"/>
-      <c r="D57" s="66"/>
-      <c r="E57" s="58"/>
-      <c r="F57" s="64"/>
-      <c r="G57" s="58"/>
-    </row>
-    <row r="58" spans="1:7" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="58"/>
-      <c r="B58" s="58"/>
-      <c r="C58" s="58"/>
-      <c r="D58" s="66"/>
-      <c r="E58" s="58"/>
-      <c r="F58" s="61"/>
-      <c r="G58" s="58"/>
-    </row>
-    <row r="59" spans="1:7" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A59" s="58"/>
-      <c r="B59" s="58"/>
-      <c r="C59" s="58"/>
-      <c r="D59" s="61"/>
-      <c r="E59" s="67"/>
-      <c r="F59" s="61"/>
-      <c r="G59" s="61"/>
-    </row>
-    <row r="60" spans="1:7" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="58"/>
-      <c r="B60" s="58"/>
-      <c r="C60" s="58"/>
-      <c r="D60" s="61"/>
-      <c r="E60" s="67"/>
-      <c r="F60" s="61"/>
-      <c r="G60" s="61"/>
-    </row>
-    <row r="61" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="58"/>
-      <c r="B61" s="68"/>
-      <c r="C61" s="68"/>
-      <c r="D61" s="68"/>
-      <c r="E61" s="68"/>
-      <c r="F61" s="69"/>
-      <c r="G61" s="58"/>
+    <row r="51" spans="1:7" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51" s="33"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="33"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="33"/>
+      <c r="F51" s="34"/>
+      <c r="G51" s="33"/>
+    </row>
+    <row r="52" spans="1:7" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A52" s="33"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="33"/>
+      <c r="D52" s="34"/>
+      <c r="E52" s="33"/>
+      <c r="F52" s="34"/>
+      <c r="G52" s="33"/>
+    </row>
+    <row r="53" spans="1:7" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="33"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="33"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="33"/>
+      <c r="F53" s="34"/>
+      <c r="G53" s="33"/>
+    </row>
+    <row r="54" spans="1:7" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="33"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="33"/>
+      <c r="D54" s="34"/>
+      <c r="E54" s="33"/>
+      <c r="F54" s="35"/>
+      <c r="G54" s="33"/>
+    </row>
+    <row r="55" spans="1:7" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55" s="33"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="33"/>
+      <c r="D55" s="34"/>
+      <c r="E55" s="33"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="33"/>
+    </row>
+    <row r="56" spans="1:7" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A56" s="33"/>
+      <c r="B56" s="12"/>
+      <c r="C56" s="33"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="33"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="33"/>
+    </row>
+    <row r="57" spans="1:7" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A57" s="33"/>
+      <c r="B57" s="12"/>
+      <c r="C57" s="33"/>
+      <c r="D57" s="57"/>
+      <c r="E57" s="33"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="33"/>
+    </row>
+    <row r="58" spans="1:7" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" s="33"/>
+      <c r="B58" s="33"/>
+      <c r="C58" s="33"/>
+      <c r="D58" s="57"/>
+      <c r="E58" s="33"/>
+      <c r="F58" s="34"/>
+      <c r="G58" s="33"/>
+    </row>
+    <row r="59" spans="1:7" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A59" s="33"/>
+      <c r="B59" s="33"/>
+      <c r="C59" s="33"/>
+      <c r="D59" s="34"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="34"/>
+      <c r="G59" s="34"/>
+    </row>
+    <row r="60" spans="1:7" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A60" s="33"/>
+      <c r="B60" s="33"/>
+      <c r="C60" s="33"/>
+      <c r="D60" s="34"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="34"/>
+      <c r="G60" s="34"/>
+    </row>
+    <row r="61" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="33"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>